<commit_message>
Update SPR valid example
</commit_message>
<xml_diff>
--- a/examples/spr-submission-valid.xlsx
+++ b/examples/spr-submission-valid.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -606,6 +606,324 @@
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>COVIC 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Nucleoprotein 1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>&gt;500000</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>23100000</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>14500</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>COVIC 1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Spike protein 2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>32100</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>6100</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>14.6</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>COVIC 4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Nucleoprotein 1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>&gt;500000</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>&gt;200000000</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>COVIC 4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Spike protein 1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>674000</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>12.3</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>COVIC 10</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Spike protein 2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>&gt;500000</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>&gt;200000000</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>COVIC 10</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Nucleoprotein 1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>82000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>&lt;.1</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Fix ab_label to ab_id switch
</commit_message>
<xml_diff>
--- a/examples/spr-submission-valid.xlsx
+++ b/examples/spr-submission-valid.xlsx
@@ -943,7 +943,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>COVIC-10</t>
+          <t>isotype control</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -996,7 +996,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="J2:J100" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>=Terminology!$A$2:$A$4</formula1>
+      <formula1>=Terminology!$A$2:$A$7</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1009,7 +1009,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1049,6 +1049,27 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>weak</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>strong</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>